<commit_message>
2023 TUCP zooplankton graphs and 2022 updates to fish graphs
</commit_message>
<xml_diff>
--- a/data/zoopcrosswalk.xlsx
+++ b/data/zoopcrosswalk.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cawater-my.sharepoint.com/personal/rosemary_hartman_water_ca_gov/Documents/Drought/DroughtSynthesis/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cawater-my.sharepoint.com/personal/rosemary_hartman_water_ca_gov/Documents/Drought/Barrier/EDB-Effectiveness/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7C6A1AD2-CF8D-4574-98FB-EE3CE1ACF9B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="8_{7C6A1AD2-CF8D-4574-98FB-EE3CE1ACF9B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{69B9C293-177A-46E9-A57C-2AA1FF0A0067}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{21022F0F-4E86-4209-95BA-C8F35D0B1478}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{21022F0F-4E86-4209-95BA-C8F35D0B1478}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="984" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="998" uniqueCount="112">
   <si>
     <t>Taxname</t>
   </si>
@@ -367,6 +367,9 @@
   </si>
   <si>
     <t>Macrocyclops albidus</t>
+  </si>
+  <si>
+    <t>Daphniidae</t>
   </si>
 </sst>
 </file>
@@ -719,10 +722,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A5219F6-672F-4E42-B512-BEBCEEFE4775}">
-  <dimension ref="A1:G142"/>
+  <dimension ref="A1:G144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" topLeftCell="B118" workbookViewId="0">
+      <selection activeCell="G144" sqref="G144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3972,6 +3975,52 @@
         <v>19</v>
       </c>
     </row>
+    <row r="143" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A143" t="s">
+        <v>111</v>
+      </c>
+      <c r="B143" t="s">
+        <v>14</v>
+      </c>
+      <c r="C143" t="s">
+        <v>9</v>
+      </c>
+      <c r="D143" t="s">
+        <v>27</v>
+      </c>
+      <c r="E143" t="s">
+        <v>28</v>
+      </c>
+      <c r="F143" t="s">
+        <v>28</v>
+      </c>
+      <c r="G143" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A144" t="s">
+        <v>12</v>
+      </c>
+      <c r="B144" t="s">
+        <v>35</v>
+      </c>
+      <c r="C144" t="s">
+        <v>9</v>
+      </c>
+      <c r="D144" t="s">
+        <v>10</v>
+      </c>
+      <c r="E144" t="s">
+        <v>11</v>
+      </c>
+      <c r="F144" t="s">
+        <v>11</v>
+      </c>
+      <c r="G144" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>